<commit_message>
updated H1 and titke tag
</commit_message>
<xml_diff>
--- a/task-excel-export/InputFile.xlsx
+++ b/task-excel-export/InputFile.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aravind.jayanna\Desktop\upload\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Aravind-jayanna\DI_Onboarding\task-excel-export\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB64C55D-12B1-44CC-975E-B524CCD35A25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9B77FA-6124-4429-8AE9-FFCF57307E60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3490" yWindow="2580" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -96,13 +96,13 @@
     <t>Design</t>
   </si>
   <si>
-    <t>xyz</t>
-  </si>
-  <si>
     <t>15/10/1992</t>
   </si>
   <si>
     <t>sales</t>
+  </si>
+  <si>
+    <t>surya</t>
   </si>
 </sst>
 </file>
@@ -443,7 +443,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD18"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -729,16 +729,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="C17" s="6">
         <v>167</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E17" s="7">
         <v>60600</v>

</xml_diff>